<commit_message>
momentum, backprop, CV, FCT
Added in backprop, momentum, and the hidden layer. CV for free parameters. Forced choice test cases for ortho to phono
</commit_message>
<xml_diff>
--- a/cRep.xlsx
+++ b/cRep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenahblack/Documents/School/College/Research/Thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35099D9B-2BA5-B444-A1B9-C54BEC21EFC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A271CCF-154A-B346-B252-3E2EBC3D5F0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="1960" windowWidth="26840" windowHeight="15540" xr2:uid="{E222ABF8-8EDC-634E-9D16-E290EB8F6BB7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>CMUPD</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>radical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diphthong </t>
   </si>
 </sst>
 </file>
@@ -485,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6475AC7-7FDD-0C4B-A529-F179B3B8FA8E}">
-  <dimension ref="A1:Y12"/>
+  <dimension ref="A1:Y13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:Y13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1417,6 +1420,83 @@
         <v>1</v>
       </c>
     </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>